<commit_message>
added Day 8 - Hands On Demos
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Training\Virtual Training\ACE\Coforge\Angular - Spring Boot - Microservices With Spring Cloud\Setup and Installation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB3313A-EE58-4BB5-B71D-47CA21008E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Setup" sheetId="1" r:id="rId1"/>
@@ -32,6 +26,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>JDK 11 (or 17)</t>
   </si>
   <si>
     <t>https://www.oracle.com/in/java/technologies/javase/jdk11-archive-downloads.html</t>
@@ -77,6 +74,72 @@
     <t>http://git-scm.com/download/win</t>
   </si>
   <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>https://github.com/join</t>
+  </si>
+  <si>
+    <t>Sign up  for a GitHub account</t>
+  </si>
+  <si>
+    <t>Microsoft VSCode version 1.62.2 or later</t>
+  </si>
+  <si>
+    <t>https://code.visualstudio.com/download</t>
+  </si>
+  <si>
+    <t>Node.js</t>
+  </si>
+  <si>
+    <t>https://nodejs.org/en/download/</t>
+  </si>
+  <si>
+    <t>Apache Maven 3.8.4</t>
+  </si>
+  <si>
+    <t>https://maven.apache.org/download.cgi</t>
+  </si>
+  <si>
+    <t>Spring Tool Suite 4</t>
+  </si>
+  <si>
+    <t>https://spring.io/tools/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Refer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spring Tool Suite - Setup and Installation.pptx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 'Setup and Installation' folder.</t>
+    </r>
+  </si>
+  <si>
     <t>MySQL Community Server 8.0</t>
   </si>
   <si>
@@ -123,110 +186,40 @@
     <t>https://www.postman.com/downloads/</t>
   </si>
   <si>
-    <t>Microsoft VSCode version 1.62.2 or later</t>
-  </si>
-  <si>
-    <t>https://code.visualstudio.com/download</t>
-  </si>
-  <si>
-    <t>Node.js</t>
-  </si>
-  <si>
-    <t>https://nodejs.org/en/download/</t>
-  </si>
-  <si>
-    <t>GitHub</t>
-  </si>
-  <si>
-    <t>https://github.com/join</t>
-  </si>
-  <si>
-    <t>Sign up  for a GitHub account</t>
-  </si>
-  <si>
-    <t>Spring Tool Suite 4</t>
-  </si>
-  <si>
-    <t>https://spring.io/tools/</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Refer </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Spring Tool Suite - Setup and Installation.pptx</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in 'Setup and Installation' folder.</t>
-    </r>
-  </si>
-  <si>
     <t>Keycloak</t>
   </si>
   <si>
+    <t>https://www.keycloak.org/getting-started/getting-started-zip</t>
+  </si>
+  <si>
     <t>Only download keycloak-21.1.1.zip from the website.</t>
   </si>
   <si>
-    <t>https://www.keycloak.org/getting-started/getting-started-zip</t>
-  </si>
-  <si>
     <t>Docker Desktop</t>
   </si>
   <si>
     <t>https://www.docker.com/get-started/</t>
   </si>
   <si>
-    <t>JDK 11 (or 17)</t>
-  </si>
-  <si>
     <t>Install Docker Desktop and Sign up for Docker Hub @ the same URL</t>
-  </si>
-  <si>
-    <t>Apache Maven 3.8.4</t>
-  </si>
-  <si>
-    <t>https://maven.apache.org/download.cgi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,6 +250,7 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -270,6 +264,163 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,32 +437,205 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -319,59 +643,338 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -629,28 +1232,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" customWidth="1"/>
+    <col min="3" max="3" width="76.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" ht="18.75" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,186 +1268,186 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.75">
+    <row r="3" ht="30" spans="1:4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>28</v>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" ht="18.75" spans="1:3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="18.75" spans="1:3">
       <c r="A6" s="2"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75">
+    <row r="7" ht="18.75" spans="1:4">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="18.75">
+    <row r="9" ht="18.75" spans="1:3">
       <c r="A9" s="2">
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75">
+    <row r="11" ht="18.75" spans="1:3">
       <c r="A11" s="2">
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="18.75">
+    <row r="13" ht="18.75" spans="1:3">
       <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>30</v>
+      <c r="B13" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="30.75">
+    <row r="15" ht="30" spans="1:4">
       <c r="A15" s="2">
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18.75">
+    </row>
+    <row r="16" ht="18.75" spans="1:2">
       <c r="A16" s="2"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="30.75">
+    <row r="17" ht="30" spans="1:4">
       <c r="A17" s="2">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+      <c r="B17" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" spans="1:3">
       <c r="A19" s="2">
         <v>9</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="18.75">
+    <row r="21" ht="18.75" spans="1:4">
       <c r="A21" s="2">
         <v>10</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>23</v>
+      <c r="B21" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30.75">
+        <v>27</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" ht="30" spans="1:4">
       <c r="A23" s="2">
         <v>11</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>26</v>
+      <c r="B23" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="18.75">
+        <v>30</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75" spans="1:3">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" ht="18.75">
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" ht="18.75" spans="1:3">
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="27" ht="17.1" customHeight="1" spans="1:3">
       <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="7"/>
     </row>
     <row r="29" spans="1:4">
@@ -861,18 +1465,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C19" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{0589BD46-8B99-4008-8DBD-21E48EDDDF34}"/>
-    <hyperlink ref="C15" r:id="rId8" xr:uid="{97173FFC-41D4-45CC-9526-FF55CA853027}"/>
-    <hyperlink ref="C21" r:id="rId9" xr:uid="{34CBC495-D754-44E8-85EC-C81A21240AA8}"/>
-    <hyperlink ref="C23" r:id="rId10" xr:uid="{523717F8-24C5-42D0-969A-76875F6F8129}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.oracle.com/in/java/technologies/javase/jdk11-archive-downloads.html"/>
+    <hyperlink ref="C5" r:id="rId2" display="http://git-scm.com/download/win"/>
+    <hyperlink ref="C17" r:id="rId3" display="https://dev.mysql.com/downloads/mysql/"/>
+    <hyperlink ref="C11" r:id="rId4" display="https://nodejs.org/en/download/"/>
+    <hyperlink ref="C9" r:id="rId5" display="https://code.visualstudio.com/download"/>
+    <hyperlink ref="C19" r:id="rId6" display="https://www.postman.com/downloads/"/>
+    <hyperlink ref="C7" r:id="rId7" display="https://github.com/join"/>
+    <hyperlink ref="C15" r:id="rId8" display="https://spring.io/tools/"/>
+    <hyperlink ref="C21" r:id="rId9" display="https://www.keycloak.org/getting-started/getting-started-zip"/>
+    <hyperlink ref="C23" r:id="rId10" display="https://www.docker.com/get-started/"/>
+    <hyperlink ref="C13" r:id="rId11" display="https://maven.apache.org/download.cgi"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>